<commit_message>
introducing administrator staff role
</commit_message>
<xml_diff>
--- a/config/security/en_little_register.xlsx
+++ b/config/security/en_little_register.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\orokimadas\config\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7C5915F-F2CA-4671-AE5D-543F4860A173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A986FD4-2CA0-4FD4-8C68-4C8FEA9ED3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
   </bookViews>
@@ -218,7 +218,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>https://orokimadas.info</t>
+      <t>https://orokimadas.magyar.website</t>
     </r>
     <r>
       <rPr>
@@ -243,7 +243,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>https://orokimadas.info</t>
+      <t>https://orokimadas.magyar.website</t>
     </r>
   </si>
 </sst>
@@ -486,15 +486,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,6 +510,15 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,15 +541,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>93135</xdr:rowOff>
+      <xdr:colOff>375234</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>222251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1965325</xdr:colOff>
+      <xdr:colOff>2095500</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>126891</xdr:rowOff>
+      <xdr:rowOff>238600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -565,15 +565,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1121833" y="4030135"/>
-          <a:ext cx="1457325" cy="1494256"/>
+          <a:off x="989067" y="3915834"/>
+          <a:ext cx="1720266" cy="1720266"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -971,7 +976,7 @@
   <dimension ref="B2:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AG30" sqref="AG30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,33 +992,33 @@
     <row r="2" spans="2:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
@@ -1049,70 +1054,70 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" ht="61.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
     </row>
     <row r="5" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
     </row>
     <row r="6" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
@@ -1146,101 +1151,101 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
     </row>
     <row r="8" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
     </row>
     <row r="9" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="21"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
@@ -1279,32 +1284,32 @@
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
@@ -1389,7 +1394,7 @@
     </row>
     <row r="13" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1460,7 +1465,7 @@
     </row>
     <row r="14" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
@@ -1529,7 +1534,7 @@
     </row>
     <row r="15" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1598,7 +1603,7 @@
     </row>
     <row r="16" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="17"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
@@ -1667,7 +1672,7 @@
     </row>
     <row r="17" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="17"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1736,7 +1741,7 @@
     </row>
     <row r="18" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="17"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="7" t="s">
         <v>25</v>
       </c>
@@ -1805,7 +1810,7 @@
     </row>
     <row r="19" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1876,38 +1881,38 @@
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="16" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="18" t="s">
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="20" t="s">
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="22"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="18"/>
+      <c r="AA20" s="18"/>
+      <c r="AB20" s="19"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
@@ -1943,70 +1948,70 @@
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="12"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="15"/>
-      <c r="AB23" s="15"/>
-      <c r="AC23" s="15"/>
-      <c r="AD23" s="15"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="12"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -2041,6 +2046,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D2:AB2"/>
+    <mergeCell ref="B7:AD7"/>
+    <mergeCell ref="B8:AD8"/>
+    <mergeCell ref="D9:AB9"/>
+    <mergeCell ref="B5:AD5"/>
+    <mergeCell ref="B4:AD4"/>
     <mergeCell ref="B23:AD23"/>
     <mergeCell ref="B22:AD22"/>
     <mergeCell ref="E11:AB11"/>
@@ -2049,12 +2060,6 @@
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
     <mergeCell ref="W20:AB20"/>
-    <mergeCell ref="D2:AB2"/>
-    <mergeCell ref="B7:AD7"/>
-    <mergeCell ref="B8:AD8"/>
-    <mergeCell ref="D9:AB9"/>
-    <mergeCell ref="B5:AD5"/>
-    <mergeCell ref="B4:AD4"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:AB19">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
add 2 hours on Monday
</commit_message>
<xml_diff>
--- a/config/security/en_little_register.xlsx
+++ b/config/security/en_little_register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\orokimadas\config\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A986FD4-2CA0-4FD4-8C68-4C8FEA9ED3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF18ACE-501C-4FD4-8D70-74D02975789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="9915" activeTab="1" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
   </bookViews>
   <sheets>
     <sheet name="Adorálók" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -486,6 +479,15 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,15 +511,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,7 +969,7 @@
   <dimension ref="B2:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,33 +985,33 @@
     <row r="2" spans="2:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
@@ -1054,70 +1047,70 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" ht="61.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
     </row>
     <row r="5" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
     </row>
     <row r="6" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
@@ -1151,101 +1144,101 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
     </row>
     <row r="8" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
     </row>
     <row r="9" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
@@ -1284,32 +1277,32 @@
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
@@ -1394,7 +1387,7 @@
     </row>
     <row r="13" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1465,7 +1458,7 @@
     </row>
     <row r="14" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
-      <c r="C14" s="14"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
@@ -1534,7 +1527,7 @@
     </row>
     <row r="15" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
-      <c r="C15" s="14"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1603,7 +1596,7 @@
     </row>
     <row r="16" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="14"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
@@ -1672,7 +1665,7 @@
     </row>
     <row r="17" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="14"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1684,7 +1677,7 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="8" t="str">
-        <f t="shared" ref="L17:W17" si="4">IF(L44=0,"",IF(L44&gt;1,"❷","①"))</f>
+        <f t="shared" ref="L17:AA17" si="4">IF(L44=0,"",IF(L44&gt;1,"❷","①"))</f>
         <v/>
       </c>
       <c r="M17" s="8" t="str">
@@ -1731,17 +1724,29 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
+      <c r="X17" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Y17" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Z17" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AA17" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="AB17" s="10"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
     <row r="18" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="14"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="7" t="s">
         <v>25</v>
       </c>
@@ -1810,7 +1815,7 @@
     </row>
     <row r="19" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="14"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1881,38 +1886,38 @@
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="13" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="15" t="s">
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="17" t="s">
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AB20" s="19"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="22"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
@@ -1948,70 +1953,70 @@
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="12"/>
-      <c r="AC22" s="12"/>
-      <c r="AD22" s="12"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="12"/>
-      <c r="AC23" s="12"/>
-      <c r="AD23" s="12"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="15"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -2046,12 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D2:AB2"/>
-    <mergeCell ref="B7:AD7"/>
-    <mergeCell ref="B8:AD8"/>
-    <mergeCell ref="D9:AB9"/>
-    <mergeCell ref="B5:AD5"/>
-    <mergeCell ref="B4:AD4"/>
     <mergeCell ref="B23:AD23"/>
     <mergeCell ref="B22:AD22"/>
     <mergeCell ref="E11:AB11"/>
@@ -2060,6 +2059,12 @@
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
     <mergeCell ref="W20:AB20"/>
+    <mergeCell ref="D2:AB2"/>
+    <mergeCell ref="B7:AD7"/>
+    <mergeCell ref="B8:AD8"/>
+    <mergeCell ref="D9:AB9"/>
+    <mergeCell ref="B5:AD5"/>
+    <mergeCell ref="B4:AD4"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:AB19">
     <cfRule type="colorScale" priority="1">

</xml_diff>